<commit_message>
Version 1.1. Fixed bug where i iterated over the wrong variable.
</commit_message>
<xml_diff>
--- a/upgrademap.xlsx
+++ b/upgrademap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Id</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>TITANIUM_MOUSE_BUTTON</t>
+  </si>
+  <si>
+    <t>LEVEL_1_SENTRY_GUN</t>
+  </si>
+  <si>
+    <t>CYBERNETIC_ENHANCEMENTS</t>
   </si>
 </sst>
 </file>
@@ -147,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -155,6 +164,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G28" sqref="G28:J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,6 +785,48 @@
         <v>10000</v>
       </c>
       <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="4">
+        <v>100000</v>
+      </c>
+      <c r="D30">
         <v>2</v>
       </c>
     </row>

</xml_diff>